<commit_message>
PSD metrics are nto working
</commit_message>
<xml_diff>
--- a/actionable_data/Clinical indicators.xlsx
+++ b/actionable_data/Clinical indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\HRV\HRV-EDA\actionable_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3FFEB0-E409-4B67-8BE2-DFD0152EA017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2172AFC-ED45-4C87-9BD9-B02AFA1CE42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="4" r:id="rId1"/>

</xml_diff>

<commit_message>
separated RR to metrics from general analysis
</commit_message>
<xml_diff>
--- a/actionable_data/Clinical indicators.xlsx
+++ b/actionable_data/Clinical indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITHUB\HRV\HRV-EDA\actionable_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01E916C-9B18-455B-951B-D808D041943D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175D677E-3FE8-45EF-A013-8ED3A4CCE46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>